<commit_message>
Update LCCV3.2 and Added 3.3
</commit_message>
<xml_diff>
--- a/Large Charging Case/LCCV3.2/LCCV3.2 BOM.xlsx
+++ b/Large Charging Case/LCCV3.2/LCCV3.2 BOM.xlsx
@@ -1,21 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\Pixels-dice\Electrical\Large Charging Case\LCCV3.2\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AA5903CB-204F-42E8-922A-B779A72DBCBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="22350" yWindow="1590" windowWidth="23910" windowHeight="18165"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -898,26 +892,26 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="等线 Light"/>
       <family val="2"/>
       <scheme val="major"/>
     </font>
@@ -925,7 +919,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -933,7 +927,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -941,35 +935,35 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -977,7 +971,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -985,14 +979,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1000,14 +994,14 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1015,7 +1009,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1023,15 +1017,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="等线"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="等线"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1381,48 +1382,48 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="标题" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="标题 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="标题 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="标题 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="标题 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="差" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="好" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="汇总" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="计算" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="检查单元格" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="解释性文本" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="警告文本" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="链接单元格" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="强调文字颜色 6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="适中" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="输出" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="输入" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="注释" xfId="15" builtinId="10" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1480,7 +1481,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1532,7 +1533,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1726,21 +1727,29 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="3" max="3" width="42.375" customWidth="1"/>
+    <col min="4" max="4" width="24.5" customWidth="1"/>
+    <col min="5" max="5" width="48.25" customWidth="1"/>
+    <col min="7" max="7" width="19.875" customWidth="1"/>
+    <col min="8" max="8" width="24.25" customWidth="1"/>
+    <col min="9" max="9" width="33.75" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1748,7 +1757,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1756,7 +1765,7 @@
         <v>44969.8512962963</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1788,7 +1797,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1814,7 +1823,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1843,7 +1852,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>3</v>
       </c>
@@ -1872,7 +1881,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>4</v>
       </c>
@@ -1904,7 +1913,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>5</v>
       </c>
@@ -1936,7 +1945,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>6</v>
       </c>
@@ -1965,7 +1974,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>7</v>
       </c>
@@ -1994,7 +2003,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>8</v>
       </c>
@@ -2023,7 +2032,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>9</v>
       </c>
@@ -2052,7 +2061,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>10</v>
       </c>
@@ -2084,7 +2093,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10">
       <c r="A15">
         <v>11</v>
       </c>
@@ -2116,7 +2125,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10">
       <c r="A16">
         <v>12</v>
       </c>
@@ -2145,7 +2154,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>13</v>
       </c>
@@ -2168,7 +2177,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>14</v>
       </c>
@@ -2197,7 +2206,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>15</v>
       </c>
@@ -2226,7 +2235,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>16</v>
       </c>
@@ -2243,7 +2252,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>17</v>
       </c>
@@ -2260,7 +2269,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>18</v>
       </c>
@@ -2277,7 +2286,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10">
       <c r="A23">
         <v>19</v>
       </c>
@@ -2306,7 +2315,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10">
       <c r="A24">
         <v>20</v>
       </c>
@@ -2329,7 +2338,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10">
       <c r="A25">
         <v>21</v>
       </c>
@@ -2361,7 +2370,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10">
       <c r="A26">
         <v>22</v>
       </c>
@@ -2390,7 +2399,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10">
       <c r="A27">
         <v>23</v>
       </c>
@@ -2416,7 +2425,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10">
       <c r="A28">
         <v>24</v>
       </c>
@@ -2445,7 +2454,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10">
       <c r="A29">
         <v>25</v>
       </c>
@@ -2471,7 +2480,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10">
       <c r="A30">
         <v>26</v>
       </c>
@@ -2488,7 +2497,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10">
       <c r="A31">
         <v>27</v>
       </c>
@@ -2517,7 +2526,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10">
       <c r="A32">
         <v>28</v>
       </c>
@@ -2546,7 +2555,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10">
       <c r="A33">
         <v>29</v>
       </c>
@@ -2575,7 +2584,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10">
       <c r="A34">
         <v>30</v>
       </c>
@@ -2604,7 +2613,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10">
       <c r="A35">
         <v>31</v>
       </c>
@@ -2630,7 +2639,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10">
       <c r="A36">
         <v>32</v>
       </c>
@@ -2656,7 +2665,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10">
       <c r="A37">
         <v>33</v>
       </c>
@@ -2685,7 +2694,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10">
       <c r="A38">
         <v>34</v>
       </c>
@@ -2714,7 +2723,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10">
       <c r="A39">
         <v>35</v>
       </c>
@@ -2743,7 +2752,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10">
       <c r="A40">
         <v>36</v>
       </c>
@@ -2772,7 +2781,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10">
       <c r="A41">
         <v>37</v>
       </c>
@@ -2804,7 +2813,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10">
       <c r="A42">
         <v>38</v>
       </c>
@@ -2836,7 +2845,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10">
       <c r="A43">
         <v>39</v>
       </c>
@@ -2865,7 +2874,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10">
       <c r="A44">
         <v>40</v>
       </c>
@@ -2894,7 +2903,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10">
       <c r="A45">
         <v>41</v>
       </c>
@@ -2923,7 +2932,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10">
       <c r="A46">
         <v>42</v>
       </c>
@@ -2949,7 +2958,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10">
       <c r="A47">
         <v>43</v>
       </c>
@@ -2975,7 +2984,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10">
       <c r="A48">
         <v>44</v>
       </c>
@@ -2998,7 +3007,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9">
       <c r="A49">
         <v>45</v>
       </c>
@@ -3024,7 +3033,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9">
       <c r="A50">
         <v>46</v>
       </c>
@@ -3050,7 +3059,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9">
       <c r="A51">
         <v>47</v>
       </c>
@@ -3076,7 +3085,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9">
       <c r="A52">
         <v>48</v>
       </c>
@@ -3099,7 +3108,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9">
       <c r="A53">
         <v>49</v>
       </c>
@@ -3125,7 +3134,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9">
       <c r="A54">
         <v>50</v>
       </c>
@@ -3142,7 +3151,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9">
       <c r="A55">
         <v>51</v>
       </c>
@@ -3159,7 +3168,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9">
       <c r="A56">
         <v>52</v>
       </c>
@@ -3176,7 +3185,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9">
       <c r="A57">
         <v>53</v>
       </c>
@@ -3193,7 +3202,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9">
       <c r="A58">
         <v>54</v>
       </c>
@@ -3210,7 +3219,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9">
       <c r="A59">
         <v>55</v>
       </c>
@@ -3227,7 +3236,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9">
       <c r="A60">
         <v>56</v>
       </c>
@@ -3244,7 +3253,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9">
       <c r="A61">
         <v>57</v>
       </c>
@@ -3261,7 +3270,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9">
       <c r="A62">
         <v>58</v>
       </c>
@@ -3278,7 +3287,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9">
       <c r="A63">
         <v>59</v>
       </c>
@@ -3295,7 +3304,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9">
       <c r="A64">
         <v>60</v>
       </c>
@@ -3312,7 +3321,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>61</v>
       </c>
@@ -3329,7 +3338,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>62</v>
       </c>
@@ -3346,7 +3355,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>63</v>
       </c>
@@ -3363,7 +3372,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>64</v>
       </c>
@@ -3380,7 +3389,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>65</v>
       </c>
@@ -3397,7 +3406,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>66</v>
       </c>
@@ -3414,7 +3423,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>67</v>
       </c>
@@ -3431,7 +3440,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10">
       <c r="A72">
         <v>68</v>
       </c>
@@ -3448,7 +3457,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10">
       <c r="A73">
         <v>69</v>
       </c>
@@ -3465,7 +3474,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10">
       <c r="A74">
         <v>70</v>
       </c>
@@ -3482,7 +3491,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10">
       <c r="A75">
         <v>71</v>
       </c>
@@ -3515,6 +3524,8 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="256" orientation="portrait" horizontalDpi="203" verticalDpi="203" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>